<commit_message>
-Selected components for 13mm mated stacking height -Fixed the lower mezzanine connector (replaced with receptacle) -Updated BOM file and added standoffs
</commit_message>
<xml_diff>
--- a/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
+++ b/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>Item #</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Keystone</t>
   </si>
   <si>
-    <t>TP1, TP2, TP11</t>
-  </si>
-  <si>
     <t>TESTPOINT-YELLOW</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marote - Breakout Board (Rev A)'</t>
-  </si>
-  <si>
-    <t>J1, J2</t>
   </si>
   <si>
     <t>TSW-150-08-T-D-RA</t>
@@ -136,6 +130,42 @@
       </rPr>
       <t xml:space="preserve"> The part for J3 is a 2x50 header that needs to be cut into 2x8 pieces by hand prior to assembly.</t>
     </r>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CON-71439-2164</t>
+  </si>
+  <si>
+    <t>71439-2164</t>
+  </si>
+  <si>
+    <t>WM17222-ND</t>
+  </si>
+  <si>
+    <t>CONN RECPT 64POS VERT 1MM SMD</t>
+  </si>
+  <si>
+    <t>TP1, TP2</t>
+  </si>
+  <si>
+    <t>STANDOFF</t>
+  </si>
+  <si>
+    <t>8401K-ND</t>
+  </si>
+  <si>
+    <t>STDOFF HEX M/F 4-40 .500"L ALUM</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>M1,M2,M3,M4</t>
   </si>
 </sst>
 </file>
@@ -627,16 +657,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
@@ -649,7 +679,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -706,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -730,14 +760,14 @@
         <v>19</v>
       </c>
       <c r="J4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>8.6</v>
       </c>
       <c r="L4">
         <f>J4*K4</f>
-        <v>17.2</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -745,118 +775,180 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>4.62</v>
+        <v>5.74</v>
       </c>
       <c r="L5">
         <f>J5*K5</f>
-        <v>4.62</v>
+        <v>5.74</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5009</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>0.36</v>
+        <v>4.62</v>
       </c>
       <c r="L6">
         <f>J6*K6</f>
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5009</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>0.36</v>
+      </c>
+      <c r="L7">
+        <f>J7*K7</f>
         <v>0.72</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2">
+        <v>8401</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="2">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="L8">
+        <f>J8*K8</f>
+        <v>7.17</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="6"/>
+      <c r="A10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
@@ -872,7 +964,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
@@ -888,31 +980,31 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="H14"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="H15"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="J18" s="3"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -922,13 +1014,13 @@
       <c r="F19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+    <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
@@ -952,6 +1044,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
@@ -966,7 +1059,6 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -984,22 +1076,22 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -1106,7 +1198,7 @@
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
+      <c r="B43" s="1"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1129,13 +1221,13 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
@@ -1209,34 +1301,31 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="8"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="3"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
@@ -1260,13 +1349,24 @@
       <c r="I61" s="9"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I62" s="7"/>
+    <row r="62" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I63" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated BOM and added new datasheets.
</commit_message>
<xml_diff>
--- a/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
+++ b/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>Item #</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marote - Breakout Board (Rev A)'</t>
+  </si>
+  <si>
+    <t>TSW-150-08-T-D-RA</t>
+  </si>
+  <si>
+    <t>SAM1049-50-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADR 100PS .100 DL R/A TIN</t>
   </si>
   <si>
     <t>CON-2X8</t>
@@ -409,7 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,6 +496,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -793,7 +805,7 @@
   <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>13</v>
@@ -909,28 +921,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J5" s="17">
         <v>1</v>
@@ -938,8 +950,8 @@
       <c r="K5">
         <v>5.74</v>
       </c>
-      <c r="L5">
-        <f>J5*K5</f>
+      <c r="L5" s="30">
+        <f t="shared" ref="L5:L14" si="0">J5*K5</f>
         <v>5.74</v>
       </c>
     </row>
@@ -948,13 +960,38 @@
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>11</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1</v>
+      </c>
+      <c r="K6" s="30">
+        <v>4.62</v>
+      </c>
+      <c r="L6" s="30">
+        <f t="shared" si="0"/>
+        <v>4.62</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -962,28 +999,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J7" s="17">
         <v>1</v>
@@ -991,8 +1028,8 @@
       <c r="K7">
         <v>1.66</v>
       </c>
-      <c r="L7" s="20">
-        <f>J7*K7</f>
+      <c r="L7" s="30">
+        <f t="shared" si="0"/>
         <v>1.66</v>
       </c>
     </row>
@@ -1001,28 +1038,28 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C8" s="17">
         <v>10</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J8" s="17">
         <v>10</v>
@@ -1030,8 +1067,8 @@
       <c r="K8" s="19">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="L8" s="19">
-        <f>J8*K8</f>
+      <c r="L8" s="30">
+        <f t="shared" si="0"/>
         <v>0.42000000000000004</v>
       </c>
     </row>
@@ -1040,28 +1077,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C9" s="17">
         <v>0</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J9" s="17">
         <v>21</v>
@@ -1070,7 +1107,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="L9" s="19">
-        <f>J9*K9</f>
+        <f t="shared" si="0"/>
         <v>0.86099999999999999</v>
       </c>
     </row>
@@ -1079,28 +1116,28 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G10" s="23" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J10" s="17">
         <v>5</v>
@@ -1108,8 +1145,8 @@
       <c r="K10">
         <v>0.99</v>
       </c>
-      <c r="L10">
-        <f>J10*K10</f>
+      <c r="L10" s="30">
+        <f t="shared" si="0"/>
         <v>4.95</v>
       </c>
     </row>
@@ -1118,13 +1155,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>20</v>
@@ -1136,10 +1173,10 @@
         <v>11</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J11" s="17">
         <v>6</v>
@@ -1147,8 +1184,8 @@
       <c r="K11">
         <v>0.38</v>
       </c>
-      <c r="L11">
-        <f>J11*K11</f>
+      <c r="L11" s="30">
+        <f t="shared" si="0"/>
         <v>2.2800000000000002</v>
       </c>
     </row>
@@ -1157,13 +1194,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>20</v>
@@ -1175,10 +1212,10 @@
         <v>11</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J12" s="17">
         <v>4</v>
@@ -1186,8 +1223,8 @@
       <c r="K12" s="20">
         <v>0.38</v>
       </c>
-      <c r="L12" s="20">
-        <f>J12*K12</f>
+      <c r="L12" s="30">
+        <f t="shared" si="0"/>
         <v>1.52</v>
       </c>
     </row>
@@ -1196,7 +1233,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>17</v>
@@ -1225,8 +1262,8 @@
       <c r="K13">
         <v>0.36</v>
       </c>
-      <c r="L13">
-        <f>J13*K13</f>
+      <c r="L13" s="30">
+        <f t="shared" si="0"/>
         <v>1.44</v>
       </c>
     </row>
@@ -1235,13 +1272,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>20</v>
@@ -1253,10 +1290,10 @@
         <v>11</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J14" s="17">
         <v>10</v>
@@ -1264,8 +1301,8 @@
       <c r="K14">
         <v>0.71699999999999997</v>
       </c>
-      <c r="L14">
-        <f>J14*K14</f>
+      <c r="L14" s="30">
+        <f t="shared" si="0"/>
         <v>7.17</v>
       </c>
     </row>
@@ -1279,7 +1316,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>

</xml_diff>

<commit_message>
Updated the BOM file.
</commit_message>
<xml_diff>
--- a/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
+++ b/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
@@ -856,7 +856,7 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,13 +1030,13 @@
       <c r="C6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="14" t="s">

</xml_diff>

<commit_message>
Updated connector names and BOM file.
</commit_message>
<xml_diff>
--- a/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
+++ b/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="80">
   <si>
     <t>Item #</t>
   </si>
@@ -102,7 +102,145 @@
     <t>CON-2X8</t>
   </si>
   <si>
-    <t>J3*</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CON-71439-2164</t>
+  </si>
+  <si>
+    <t>71439-2164</t>
+  </si>
+  <si>
+    <t>WM17222-ND</t>
+  </si>
+  <si>
+    <t>CONN RECPT 64POS VERT 1MM SMD</t>
+  </si>
+  <si>
+    <t>STANDOFF</t>
+  </si>
+  <si>
+    <t>8401K-ND</t>
+  </si>
+  <si>
+    <t>STDOFF HEX M/F 4-40 .500"L ALUM</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>R5, R10, R15, R20, R25</t>
+  </si>
+  <si>
+    <t>R1, R4, R6, R9, R11, R14, R16, R19, R21, R24</t>
+  </si>
+  <si>
+    <t>CON-HTST-105-04-D-RA</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>R0805</t>
+  </si>
+  <si>
+    <t>Rohm</t>
+  </si>
+  <si>
+    <t>Panasonic - ECG</t>
+  </si>
+  <si>
+    <t>P3W102CT-ND</t>
+  </si>
+  <si>
+    <t>EVM-3WSX80B13</t>
+  </si>
+  <si>
+    <t>TRIMMER 1K OHM 0.15W SMD</t>
+  </si>
+  <si>
+    <t>3 mm Square Low-Profi le SMT</t>
+  </si>
+  <si>
+    <t>MCR10EZPF10R0</t>
+  </si>
+  <si>
+    <t>RHM10.0CRCT-ND</t>
+  </si>
+  <si>
+    <t>RES 10.0 OHM 1/8W 1% 0805 SMD</t>
+  </si>
+  <si>
+    <t>MCR10EZHJ000</t>
+  </si>
+  <si>
+    <t>RHM0.0ACT-ND</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/8W 0805 SMD</t>
+  </si>
+  <si>
+    <t>TSW-105-08-G-D-RA</t>
+  </si>
+  <si>
+    <t>SAM1037-05-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER 10POS .100 DL R/A AU</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6</t>
+  </si>
+  <si>
+    <t>TESTPOINT-BLUE</t>
+  </si>
+  <si>
+    <t>TESTPOINT-GREEN</t>
+  </si>
+  <si>
+    <t>TP7, TP8, TP9, TP10</t>
+  </si>
+  <si>
+    <t>TP11, TP12, TP13, TP14</t>
+  </si>
+  <si>
+    <t>5122K-ND</t>
+  </si>
+  <si>
+    <t>5121K-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT T/H GREEN</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT T/H BLUE</t>
+  </si>
+  <si>
+    <t>R2, R3, R7, R8, R12, R13, R17, R18, R22, R23, R26, R27, R28, R29, R30, R31, R32, R33, R34</t>
+  </si>
+  <si>
+    <t>Qty per board</t>
+  </si>
+  <si>
+    <t>Total Qty</t>
+  </si>
+  <si>
+    <t>Number of boards:</t>
+  </si>
+  <si>
+    <t>MCR10ERTF20R0</t>
+  </si>
+  <si>
+    <t>RHM20.0CRCT-ND</t>
+  </si>
+  <si>
+    <t>RES 20.0 OHM 1/8W 1% 0805 SMD</t>
+  </si>
+  <si>
+    <t>J3, J4, J5, J6*</t>
   </si>
   <si>
     <r>
@@ -125,155 +263,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> The part for J3 is a 2x50 header that needs to be cut into 2x8 pieces by hand prior to assembly.</t>
+      <t xml:space="preserve"> The part for J3, J4, J5 and J6 is a 2x50 header that needs to be cut into 2x8 pieces by hand prior to assembling.</t>
     </r>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>CON-71439-2164</t>
-  </si>
-  <si>
-    <t>71439-2164</t>
-  </si>
-  <si>
-    <t>WM17222-ND</t>
-  </si>
-  <si>
-    <t>CONN RECPT 64POS VERT 1MM SMD</t>
-  </si>
-  <si>
-    <t>STANDOFF</t>
-  </si>
-  <si>
-    <t>8401K-ND</t>
-  </si>
-  <si>
-    <t>STDOFF HEX M/F 4-40 .500"L ALUM</t>
-  </si>
-  <si>
-    <t>Aluminum</t>
-  </si>
-  <si>
-    <t>M1,M2,M3,M4</t>
-  </si>
-  <si>
-    <t>R5, R10, R15, R20, R25</t>
-  </si>
-  <si>
-    <t>R1, R4, R6, R9, R11, R14, R16, R19, R21, R24</t>
-  </si>
-  <si>
-    <t>CON-HTST-105-04-D-RA</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>Rohm</t>
-  </si>
-  <si>
-    <t>Panasonic - ECG</t>
-  </si>
-  <si>
-    <t>P3W102CT-ND</t>
-  </si>
-  <si>
-    <t>EVM-3WSX80B13</t>
-  </si>
-  <si>
-    <t>TRIMMER 1K OHM 0.15W SMD</t>
-  </si>
-  <si>
-    <t>3 mm Square Low-Profi le SMT</t>
-  </si>
-  <si>
-    <t>MCR10EZPF10R0</t>
-  </si>
-  <si>
-    <t>RHM10.0CRCT-ND</t>
-  </si>
-  <si>
-    <t>RES 10.0 OHM 1/8W 1% 0805 SMD</t>
-  </si>
-  <si>
-    <t>MCR10EZHJ000</t>
-  </si>
-  <si>
-    <t>RHM0.0ACT-ND</t>
-  </si>
-  <si>
-    <t>RES 0.0 OHM 1/8W 0805 SMD</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>TSW-105-08-G-D-RA</t>
-  </si>
-  <si>
-    <t>SAM1037-05-ND</t>
-  </si>
-  <si>
-    <t>CONN HEADER 10POS .100 DL R/A AU</t>
-  </si>
-  <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6</t>
-  </si>
-  <si>
-    <t>TESTPOINT-BLUE</t>
-  </si>
-  <si>
-    <t>TESTPOINT-GREEN</t>
-  </si>
-  <si>
-    <t>TP7, TP8, TP9, TP10</t>
-  </si>
-  <si>
-    <t>TP11, TP12, TP13, TP14</t>
-  </si>
-  <si>
-    <t>5122K-ND</t>
-  </si>
-  <si>
-    <t>5121K-ND</t>
-  </si>
-  <si>
-    <t>TEST POINT PC COMPACT T/H GREEN</t>
-  </si>
-  <si>
-    <t>TEST POINT PC COMPACT T/H BLUE</t>
-  </si>
-  <si>
-    <t>R2, R3, R7, R8, R12, R13, R17, R18, R22, R23, R26, R27, R28, R29, R30, R31, R32, R33, R34</t>
-  </si>
-  <si>
-    <t>Qty per board</t>
-  </si>
-  <si>
-    <t>Total Qty</t>
-  </si>
-  <si>
-    <t>Number of boards:</t>
-  </si>
-  <si>
-    <t>5*</t>
-  </si>
-  <si>
-    <t>MCR10ERTF20R0</t>
-  </si>
-  <si>
-    <t>RHM20.0CRCT-ND</t>
-  </si>
-  <si>
-    <t>RES 20.0 OHM 1/8W 1% 0805 SMD</t>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>5**</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> These are alternative parts for item 5.</t>
+    </r>
+  </si>
+  <si>
+    <t>M1, M2, M3, M4</t>
   </si>
 </sst>
 </file>
@@ -380,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -457,6 +481,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -464,7 +497,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -538,16 +571,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -855,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,21 +916,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -922,13 +961,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>17</v>
@@ -939,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>12</v>
@@ -982,28 +1021,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J5" s="14">
         <v>1</v>
@@ -1016,7 +1055,7 @@
         <v>3</v>
       </c>
       <c r="M5" s="27">
-        <f t="shared" ref="M5:M15" si="0">L5*K5</f>
+        <f>L5*K5</f>
         <v>17.22</v>
       </c>
     </row>
@@ -1025,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>27</v>
@@ -1055,11 +1094,11 @@
         <v>4.62</v>
       </c>
       <c r="L6" s="28">
-        <f>J6*$C$21</f>
+        <f t="shared" ref="L6:L15" si="0">J6*$C$21</f>
         <v>3</v>
       </c>
       <c r="M6" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M6:M15" si="1">L6*K6</f>
         <v>13.86</v>
       </c>
     </row>
@@ -1068,28 +1107,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J7" s="14">
         <v>1</v>
@@ -1098,11 +1137,11 @@
         <v>1.66</v>
       </c>
       <c r="L7" s="28">
-        <f>J7*$C$21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M7" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9799999999999995</v>
       </c>
     </row>
@@ -1111,28 +1150,28 @@
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="14">
         <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J8" s="14">
         <v>10</v>
@@ -1141,41 +1180,41 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="L8" s="28">
-        <f>J8*$C$21</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="M8" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="14">
+        <v>20</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="14">
-        <v>10</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>45</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J9" s="14">
         <v>10</v>
@@ -1184,11 +1223,11 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="L9" s="28">
-        <f>J9*$C$21</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="M9" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
     </row>
@@ -1197,28 +1236,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C10" s="14">
         <v>0</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J10" s="14">
         <v>19</v>
@@ -1227,11 +1266,11 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="L10" s="28">
-        <f>J10*$C$21</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="M10" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3370000000000002</v>
       </c>
     </row>
@@ -1240,28 +1279,28 @@
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="D11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J11" s="14">
         <v>5</v>
@@ -1270,11 +1309,11 @@
         <v>0.99</v>
       </c>
       <c r="L11" s="28">
-        <f>J11*$C$21</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="M11" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.85</v>
       </c>
     </row>
@@ -1283,13 +1322,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>19</v>
@@ -1301,10 +1340,10 @@
         <v>10</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J12" s="14">
         <v>6</v>
@@ -1313,11 +1352,11 @@
         <v>0.38</v>
       </c>
       <c r="L12" s="28">
-        <f>J12*$C$21</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="M12" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.84</v>
       </c>
     </row>
@@ -1326,13 +1365,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>19</v>
@@ -1344,10 +1383,10 @@
         <v>10</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J13" s="14">
         <v>4</v>
@@ -1356,11 +1395,11 @@
         <v>0.38</v>
       </c>
       <c r="L13" s="28">
-        <f>J13*$C$21</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M13" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.5600000000000005</v>
       </c>
     </row>
@@ -1369,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>16</v>
@@ -1399,11 +1438,11 @@
         <v>0.36</v>
       </c>
       <c r="L14" s="28">
-        <f>J14*$C$21</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M14" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.32</v>
       </c>
     </row>
@@ -1412,13 +1451,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>19</v>
@@ -1430,10 +1469,10 @@
         <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J15" s="14">
         <v>4</v>
@@ -1442,11 +1481,11 @@
         <v>0.71699999999999997</v>
       </c>
       <c r="L15" s="28">
-        <f>J15*$C$21</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="M15" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6039999999999992</v>
       </c>
     </row>
@@ -1457,35 +1496,44 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="M16" s="32">
+      <c r="M16" s="29">
         <f>SUM(M4:M15)</f>
         <v>105.89100000000001</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
+      <c r="A17" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="20"/>
+      <c r="A18" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
@@ -1503,11 +1551,12 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="33">
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="30">
         <v>3</v>
       </c>
       <c r="D21" s="14"/>
@@ -1914,9 +1963,11 @@
       <c r="I70" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A17:M17"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
- HW projects exported - .gwk GC-prevue files might need some extra attention
</commit_message>
<xml_diff>
--- a/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
+++ b/hardware/BreakoutBoard/BreakoutBoard_BOM.xlsx
@@ -7,9 +7,7 @@
     <workbookView xWindow="0" yWindow="150" windowWidth="23955" windowHeight="14310" tabRatio="491"/>
   </bookViews>
   <sheets>
-    <sheet name="Power Supply Board - Rev A" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Breakout Board - Rev B" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -127,9 +125,6 @@
   </si>
   <si>
     <t>TEST POINT PC COMPACT T/H BLUE</t>
-  </si>
-  <si>
-    <t>Bill of Materials for 'Marmote - Breakout Board (Rev B)'</t>
   </si>
   <si>
     <t>J3, J4, J5, J6, J7, J8, J9, J10, J11, J12, J13*</t>
@@ -211,6 +206,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Bill of Materials for 'Marmote - Breakout Board Rev B (Smoky)'</t>
   </si>
 </sst>
 </file>
@@ -815,7 +813,7 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +835,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -880,7 +878,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="28" t="s">
         <v>8</v>
@@ -891,31 +889,31 @@
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="27" t="s">
         <v>48</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>49</v>
       </c>
       <c r="J4" s="11">
         <v>1</v>
@@ -930,31 +928,31 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>44</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="J5" s="11">
         <v>1</v>
@@ -972,7 +970,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>22</v>
@@ -1012,7 +1010,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="11">
         <v>0</v>
@@ -1052,7 +1050,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>13</v>
@@ -1092,7 +1090,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>13</v>
@@ -1172,13 +1170,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="D11" s="34" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>54</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>15</v>
@@ -1190,10 +1188,10 @@
         <v>10</v>
       </c>
       <c r="H11" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="35" t="s">
         <v>55</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>56</v>
       </c>
       <c r="J11" s="34">
         <v>4</v>
@@ -1214,7 +1212,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="I12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J12" s="23">
         <f>SUM(J5:J11)</f>
@@ -1229,7 +1227,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
@@ -1666,28 +1664,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>